<commit_message>
add function support package profile
load many script at the same time
support  create new package profile
support add new package profile

automatically and save time for profile package create
</commit_message>
<xml_diff>
--- a/script_creater/5G_CDD.xlsx
+++ b/script_creater/5G_CDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\ephucle\tool_script\python\pythonlab\script_creater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7963CF91-766C-4F89-AF35-C2B363BCCE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058D3F89-95FA-46E8-B42A-C77A4D13F35E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="6" r:id="rId1"/>
@@ -887,7 +887,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1015,12 +1015,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -1834,6 +1828,27 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1862,27 +1877,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2730,17 +2724,17 @@
       <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="94"/>
-      <c r="C52" s="94"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="94"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="101"/>
       <c r="F52" s="60"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="93"/>
-      <c r="C53" s="93"/>
-      <c r="D53" s="93"/>
-      <c r="E53" s="93"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="100"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="100"/>
       <c r="F53" s="60"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2750,21 +2744,21 @@
       <c r="E54" s="64"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="95" t="s">
+      <c r="B55" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="96"/>
-      <c r="D55" s="96"/>
-      <c r="E55" s="96"/>
-      <c r="F55" s="96"/>
+      <c r="C55" s="103"/>
+      <c r="D55" s="103"/>
+      <c r="E55" s="103"/>
+      <c r="F55" s="103"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="93" t="s">
+      <c r="B56" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="93"/>
-      <c r="D56" s="93"/>
-      <c r="E56" s="93"/>
+      <c r="C56" s="100"/>
+      <c r="D56" s="100"/>
+      <c r="E56" s="100"/>
       <c r="F56" s="60"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2777,12 +2771,12 @@
       <c r="F57" s="66"/>
     </row>
     <row r="58" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="93" t="s">
+      <c r="B58" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="93"/>
-      <c r="D58" s="93"/>
-      <c r="E58" s="93"/>
+      <c r="C58" s="100"/>
+      <c r="D58" s="100"/>
+      <c r="E58" s="100"/>
       <c r="F58" s="60"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,19 +2789,19 @@
       <c r="F59" s="66"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="93" t="s">
+      <c r="B60" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
+      <c r="C60" s="100"/>
+      <c r="D60" s="100"/>
+      <c r="E60" s="100"/>
       <c r="F60" s="60"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="93"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="93"/>
+      <c r="B62" s="100"/>
+      <c r="C62" s="100"/>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
       <c r="F62" s="60"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,10 +2812,10 @@
       <c r="F63" s="66"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="93"/>
-      <c r="C64" s="93"/>
-      <c r="D64" s="93"/>
-      <c r="E64" s="93"/>
+      <c r="B64" s="100"/>
+      <c r="C64" s="100"/>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
       <c r="F64" s="60"/>
     </row>
   </sheetData>
@@ -2874,27 +2868,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="97"/>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="99" t="s">
+      <c r="A1" s="104"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="101"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="108"/>
       <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="27.6" x14ac:dyDescent="0.3">
@@ -3430,37 +3424,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
-      <c r="AB1" s="102"/>
-      <c r="AC1" s="102"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="109"/>
+      <c r="S1" s="109"/>
+      <c r="T1" s="109"/>
+      <c r="U1" s="109"/>
+      <c r="V1" s="109"/>
+      <c r="W1" s="109"/>
+      <c r="X1" s="109"/>
+      <c r="Y1" s="109"/>
+      <c r="Z1" s="109"/>
+      <c r="AA1" s="109"/>
+      <c r="AB1" s="109"/>
+      <c r="AC1" s="109"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -4000,7 +3994,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="110" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4023,7 +4017,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="103"/>
+      <c r="A3" s="110"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4032,7 +4026,7 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="103"/>
+      <c r="A4" s="110"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4052,7 +4046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4175,7 +4169,7 @@
       <c r="H3" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="104" t="s">
+      <c r="I3" s="93" t="s">
         <v>113</v>
       </c>
       <c r="J3" s="81">
@@ -4187,7 +4181,7 @@
       <c r="L3" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="104" t="s">
+      <c r="M3" s="93" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4202,7 +4196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0786183-E858-4456-B47D-9A7232EB83B8}">
   <dimension ref="A1:DE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -4216,989 +4210,989 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:109" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="95" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="106" t="s">
+      <c r="J1" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="106" t="s">
+      <c r="K1" s="95" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="106" t="s">
+      <c r="L1" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="M1" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="106" t="s">
+      <c r="N1" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="O1" s="106" t="s">
+      <c r="O1" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="106" t="s">
+      <c r="P1" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="Q1" s="106" t="s">
+      <c r="Q1" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="R1" s="106" t="s">
+      <c r="R1" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="S1" s="106" t="s">
+      <c r="S1" s="95" t="s">
         <v>135</v>
       </c>
-      <c r="T1" s="106" t="s">
+      <c r="T1" s="95" t="s">
         <v>136</v>
       </c>
-      <c r="U1" s="106" t="s">
+      <c r="U1" s="95" t="s">
         <v>137</v>
       </c>
-      <c r="V1" s="106" t="s">
+      <c r="V1" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="106" t="s">
+      <c r="W1" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="X1" s="106" t="s">
+      <c r="X1" s="95" t="s">
         <v>140</v>
       </c>
-      <c r="Y1" s="106" t="s">
+      <c r="Y1" s="95" t="s">
         <v>141</v>
       </c>
-      <c r="Z1" s="106" t="s">
+      <c r="Z1" s="95" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" s="106" t="s">
+      <c r="AA1" s="95" t="s">
         <v>143</v>
       </c>
-      <c r="AB1" s="106" t="s">
+      <c r="AB1" s="95" t="s">
         <v>144</v>
       </c>
-      <c r="AC1" s="106" t="s">
+      <c r="AC1" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="AD1" s="106" t="s">
+      <c r="AD1" s="95" t="s">
         <v>146</v>
       </c>
-      <c r="AE1" s="106" t="s">
+      <c r="AE1" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="AF1" s="106" t="s">
+      <c r="AF1" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="AG1" s="106" t="s">
+      <c r="AG1" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="AH1" s="106" t="s">
+      <c r="AH1" s="95" t="s">
         <v>150</v>
       </c>
-      <c r="AI1" s="106" t="s">
+      <c r="AI1" s="95" t="s">
         <v>151</v>
       </c>
-      <c r="AJ1" s="106" t="s">
+      <c r="AJ1" s="95" t="s">
         <v>152</v>
       </c>
-      <c r="AK1" s="106" t="s">
+      <c r="AK1" s="95" t="s">
         <v>153</v>
       </c>
-      <c r="AL1" s="106" t="s">
+      <c r="AL1" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="AM1" s="106" t="s">
+      <c r="AM1" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="AN1" s="106" t="s">
+      <c r="AN1" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="AO1" s="106" t="s">
+      <c r="AO1" s="95" t="s">
         <v>157</v>
       </c>
-      <c r="AP1" s="106" t="s">
+      <c r="AP1" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="AQ1" s="106" t="s">
+      <c r="AQ1" s="95" t="s">
         <v>159</v>
       </c>
-      <c r="AR1" s="106" t="s">
+      <c r="AR1" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="AS1" s="106" t="s">
+      <c r="AS1" s="95" t="s">
         <v>161</v>
       </c>
-      <c r="AT1" s="106" t="s">
+      <c r="AT1" s="95" t="s">
         <v>162</v>
       </c>
-      <c r="AU1" s="106" t="s">
+      <c r="AU1" s="95" t="s">
         <v>163</v>
       </c>
-      <c r="AV1" s="106" t="s">
+      <c r="AV1" s="95" t="s">
         <v>164</v>
       </c>
-      <c r="AW1" s="106" t="s">
+      <c r="AW1" s="95" t="s">
         <v>165</v>
       </c>
-      <c r="AX1" s="106" t="s">
+      <c r="AX1" s="95" t="s">
         <v>166</v>
       </c>
-      <c r="AY1" s="106" t="s">
+      <c r="AY1" s="95" t="s">
         <v>167</v>
       </c>
-      <c r="AZ1" s="106" t="s">
+      <c r="AZ1" s="95" t="s">
         <v>168</v>
       </c>
-      <c r="BA1" s="106" t="s">
+      <c r="BA1" s="95" t="s">
         <v>169</v>
       </c>
-      <c r="BB1" s="106" t="s">
+      <c r="BB1" s="95" t="s">
         <v>170</v>
       </c>
-      <c r="BC1" s="106" t="s">
+      <c r="BC1" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="BD1" s="106" t="s">
+      <c r="BD1" s="95" t="s">
         <v>172</v>
       </c>
-      <c r="BE1" s="106" t="s">
+      <c r="BE1" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="BF1" s="106" t="s">
+      <c r="BF1" s="95" t="s">
         <v>174</v>
       </c>
-      <c r="BG1" s="106" t="s">
+      <c r="BG1" s="95" t="s">
         <v>175</v>
       </c>
-      <c r="BH1" s="106" t="s">
+      <c r="BH1" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="BI1" s="106" t="s">
+      <c r="BI1" s="95" t="s">
         <v>177</v>
       </c>
-      <c r="BJ1" s="106" t="s">
+      <c r="BJ1" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="BK1" s="106" t="s">
+      <c r="BK1" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="BL1" s="106" t="s">
+      <c r="BL1" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="BM1" s="106" t="s">
+      <c r="BM1" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="BN1" s="106" t="s">
+      <c r="BN1" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="BO1" s="106" t="s">
+      <c r="BO1" s="95" t="s">
         <v>183</v>
       </c>
-      <c r="BP1" s="106" t="s">
+      <c r="BP1" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="BQ1" s="106" t="s">
+      <c r="BQ1" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="BR1" s="106" t="s">
+      <c r="BR1" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="BS1" s="106" t="s">
+      <c r="BS1" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="BT1" s="106" t="s">
+      <c r="BT1" s="95" t="s">
         <v>188</v>
       </c>
-      <c r="BU1" s="106" t="s">
+      <c r="BU1" s="95" t="s">
         <v>189</v>
       </c>
-      <c r="BV1" s="106" t="s">
+      <c r="BV1" s="95" t="s">
         <v>190</v>
       </c>
-      <c r="BW1" s="106" t="s">
+      <c r="BW1" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="BX1" s="106" t="s">
+      <c r="BX1" s="95" t="s">
         <v>192</v>
       </c>
-      <c r="BY1" s="106" t="s">
+      <c r="BY1" s="95" t="s">
         <v>193</v>
       </c>
-      <c r="BZ1" s="106" t="s">
+      <c r="BZ1" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="CA1" s="106" t="s">
+      <c r="CA1" s="95" t="s">
         <v>195</v>
       </c>
-      <c r="CB1" s="106" t="s">
+      <c r="CB1" s="95" t="s">
         <v>196</v>
       </c>
-      <c r="CC1" s="106" t="s">
+      <c r="CC1" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="CD1" s="106" t="s">
+      <c r="CD1" s="95" t="s">
         <v>198</v>
       </c>
-      <c r="CE1" s="106" t="s">
+      <c r="CE1" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="CF1" s="106" t="s">
+      <c r="CF1" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="CG1" s="106" t="s">
+      <c r="CG1" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="CH1" s="106" t="s">
+      <c r="CH1" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="CI1" s="106" t="s">
+      <c r="CI1" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="CJ1" s="106" t="s">
+      <c r="CJ1" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="CK1" s="106" t="s">
+      <c r="CK1" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="CL1" s="106" t="s">
+      <c r="CL1" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="CM1" s="106" t="s">
+      <c r="CM1" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="CN1" s="106" t="s">
+      <c r="CN1" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="CO1" s="106" t="s">
+      <c r="CO1" s="95" t="s">
         <v>209</v>
       </c>
-      <c r="CP1" s="106" t="s">
+      <c r="CP1" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="CQ1" s="106" t="s">
+      <c r="CQ1" s="95" t="s">
         <v>211</v>
       </c>
-      <c r="CR1" s="106" t="s">
+      <c r="CR1" s="95" t="s">
         <v>212</v>
       </c>
-      <c r="CS1" s="106" t="s">
+      <c r="CS1" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="CT1" s="106" t="s">
+      <c r="CT1" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="CU1" s="106" t="s">
+      <c r="CU1" s="95" t="s">
         <v>215</v>
       </c>
-      <c r="CV1" s="106" t="s">
+      <c r="CV1" s="95" t="s">
         <v>216</v>
       </c>
-      <c r="CW1" s="106" t="s">
+      <c r="CW1" s="95" t="s">
         <v>217</v>
       </c>
-      <c r="CX1" s="106" t="s">
+      <c r="CX1" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="CY1" s="106" t="s">
+      <c r="CY1" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="CZ1" s="106" t="s">
+      <c r="CZ1" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="DA1" s="106" t="s">
+      <c r="DA1" s="95" t="s">
         <v>221</v>
       </c>
-      <c r="DB1" s="106" t="s">
+      <c r="DB1" s="95" t="s">
         <v>222</v>
       </c>
-      <c r="DC1" s="106" t="s">
+      <c r="DC1" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="DD1" s="106" t="s">
+      <c r="DD1" s="95" t="s">
         <v>224</v>
       </c>
-      <c r="DE1" s="106" t="s">
+      <c r="DE1" s="95" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:109" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="107">
+      <c r="B2" s="96">
         <v>2928612</v>
       </c>
-      <c r="C2" s="107">
+      <c r="C2" s="96">
         <v>26</v>
       </c>
-      <c r="D2" s="107">
+      <c r="D2" s="96">
         <v>452</v>
       </c>
-      <c r="E2" s="109">
+      <c r="E2" s="98">
         <v>4</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="107">
+      <c r="G2" s="96">
         <v>21</v>
       </c>
-      <c r="H2" s="107">
+      <c r="H2" s="96">
         <v>258</v>
       </c>
-      <c r="I2" s="107" t="s">
+      <c r="I2" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="108">
+      <c r="J2" s="97">
         <v>26</v>
       </c>
-      <c r="K2" s="107">
+      <c r="K2" s="96">
         <v>1007</v>
       </c>
-      <c r="L2" s="107">
+      <c r="L2" s="96">
         <v>1</v>
       </c>
-      <c r="M2" s="107">
+      <c r="M2" s="96">
         <v>1</v>
       </c>
-      <c r="N2" s="107">
+      <c r="N2" s="96">
         <v>2056669</v>
       </c>
-      <c r="O2" s="107">
+      <c r="O2" s="96">
         <v>2056669</v>
       </c>
-      <c r="P2" s="107">
+      <c r="P2" s="96">
         <v>100</v>
       </c>
-      <c r="Q2" s="107">
+      <c r="Q2" s="96">
         <v>100</v>
       </c>
-      <c r="R2" s="107">
+      <c r="R2" s="96">
         <v>2056669</v>
       </c>
-      <c r="S2" s="107" t="s">
+      <c r="S2" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="T2" s="107">
+      <c r="T2" s="96">
         <v>31</v>
       </c>
-      <c r="U2" s="107">
+      <c r="U2" s="96">
         <v>258</v>
       </c>
-      <c r="V2" s="107" t="s">
+      <c r="V2" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="W2" s="108">
+      <c r="W2" s="97">
         <v>26</v>
       </c>
-      <c r="X2" s="107">
+      <c r="X2" s="96">
         <v>1006</v>
       </c>
-      <c r="Y2" s="107">
+      <c r="Y2" s="96">
         <v>1</v>
       </c>
-      <c r="Z2" s="107">
+      <c r="Z2" s="96">
         <v>1</v>
       </c>
-      <c r="AA2" s="107">
+      <c r="AA2" s="96">
         <v>2058335</v>
       </c>
-      <c r="AB2" s="107">
+      <c r="AB2" s="96">
         <v>2058335</v>
       </c>
-      <c r="AC2" s="107">
+      <c r="AC2" s="96">
         <v>100</v>
       </c>
-      <c r="AD2" s="107">
+      <c r="AD2" s="96">
         <v>100</v>
       </c>
-      <c r="AE2" s="107">
+      <c r="AE2" s="96">
         <v>2058335</v>
       </c>
-      <c r="AF2" s="107" t="s">
+      <c r="AF2" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="107">
+      <c r="AG2" s="96">
         <v>41</v>
       </c>
-      <c r="AH2" s="107">
+      <c r="AH2" s="96">
         <v>258</v>
       </c>
-      <c r="AI2" s="107" t="s">
+      <c r="AI2" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="AJ2" s="108">
+      <c r="AJ2" s="97">
         <v>26</v>
       </c>
-      <c r="AK2" s="107">
+      <c r="AK2" s="96">
         <v>1005</v>
       </c>
-      <c r="AL2" s="107">
+      <c r="AL2" s="96">
         <v>1</v>
       </c>
-      <c r="AM2" s="107">
+      <c r="AM2" s="96">
         <v>1</v>
       </c>
-      <c r="AN2" s="107">
+      <c r="AN2" s="96">
         <v>2060001</v>
       </c>
-      <c r="AO2" s="107">
+      <c r="AO2" s="96">
         <v>2060001</v>
       </c>
-      <c r="AP2" s="107">
+      <c r="AP2" s="96">
         <v>100</v>
       </c>
-      <c r="AQ2" s="107">
+      <c r="AQ2" s="96">
         <v>100</v>
       </c>
-      <c r="AR2" s="107">
+      <c r="AR2" s="96">
         <v>2060001</v>
       </c>
-      <c r="AS2" s="107" t="s">
+      <c r="AS2" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="AT2" s="107">
+      <c r="AT2" s="96">
         <v>51</v>
       </c>
-      <c r="AU2" s="107">
+      <c r="AU2" s="96">
         <v>258</v>
       </c>
-      <c r="AV2" s="107" t="s">
+      <c r="AV2" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="AW2" s="108">
+      <c r="AW2" s="97">
         <v>26</v>
       </c>
-      <c r="AX2" s="107">
+      <c r="AX2" s="96">
         <v>1004</v>
       </c>
-      <c r="AY2" s="107">
+      <c r="AY2" s="96">
         <v>1</v>
       </c>
-      <c r="AZ2" s="107">
+      <c r="AZ2" s="96">
         <v>1</v>
       </c>
-      <c r="BA2" s="107">
+      <c r="BA2" s="96">
         <v>2061667</v>
       </c>
-      <c r="BB2" s="107">
+      <c r="BB2" s="96">
         <v>2061667</v>
       </c>
-      <c r="BC2" s="107">
+      <c r="BC2" s="96">
         <v>100</v>
       </c>
-      <c r="BD2" s="107">
+      <c r="BD2" s="96">
         <v>100</v>
       </c>
-      <c r="BE2" s="107">
+      <c r="BE2" s="96">
         <v>2061667</v>
       </c>
-      <c r="BF2" s="107" t="s">
+      <c r="BF2" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="BG2" s="107">
+      <c r="BG2" s="96">
         <v>61</v>
       </c>
-      <c r="BH2" s="107">
+      <c r="BH2" s="96">
         <v>258</v>
       </c>
-      <c r="BI2" s="107" t="s">
+      <c r="BI2" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="BJ2" s="108">
+      <c r="BJ2" s="97">
         <v>26</v>
       </c>
-      <c r="BK2" s="107">
+      <c r="BK2" s="96">
         <v>1003</v>
       </c>
-      <c r="BL2" s="107">
+      <c r="BL2" s="96">
         <v>1</v>
       </c>
-      <c r="BM2" s="107">
+      <c r="BM2" s="96">
         <v>1</v>
       </c>
-      <c r="BN2" s="107">
+      <c r="BN2" s="96">
         <v>2063333</v>
       </c>
-      <c r="BO2" s="107">
+      <c r="BO2" s="96">
         <v>2063333</v>
       </c>
-      <c r="BP2" s="107">
+      <c r="BP2" s="96">
         <v>100</v>
       </c>
-      <c r="BQ2" s="107">
+      <c r="BQ2" s="96">
         <v>100</v>
       </c>
-      <c r="BR2" s="107">
+      <c r="BR2" s="96">
         <v>2063333</v>
       </c>
-      <c r="BS2" s="107" t="s">
+      <c r="BS2" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="BT2" s="107">
+      <c r="BT2" s="96">
         <v>71</v>
       </c>
-      <c r="BU2" s="107">
+      <c r="BU2" s="96">
         <v>258</v>
       </c>
-      <c r="BV2" s="107" t="s">
+      <c r="BV2" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="BW2" s="108">
+      <c r="BW2" s="97">
         <v>26</v>
       </c>
-      <c r="BX2" s="107">
+      <c r="BX2" s="96">
         <v>1002</v>
       </c>
-      <c r="BY2" s="107">
+      <c r="BY2" s="96">
         <v>1</v>
       </c>
-      <c r="BZ2" s="107">
+      <c r="BZ2" s="96">
         <v>1</v>
       </c>
-      <c r="CA2" s="107">
+      <c r="CA2" s="96">
         <v>2064999</v>
       </c>
-      <c r="CB2" s="107">
+      <c r="CB2" s="96">
         <v>2064999</v>
       </c>
-      <c r="CC2" s="107">
+      <c r="CC2" s="96">
         <v>100</v>
       </c>
-      <c r="CD2" s="107">
+      <c r="CD2" s="96">
         <v>100</v>
       </c>
-      <c r="CE2" s="107">
+      <c r="CE2" s="96">
         <v>2064999</v>
       </c>
-      <c r="CF2" s="107" t="s">
+      <c r="CF2" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="CG2" s="107">
+      <c r="CG2" s="96">
         <v>81</v>
       </c>
-      <c r="CH2" s="107">
+      <c r="CH2" s="96">
         <v>258</v>
       </c>
-      <c r="CI2" s="107" t="s">
+      <c r="CI2" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="CJ2" s="108">
+      <c r="CJ2" s="97">
         <v>26</v>
       </c>
-      <c r="CK2" s="107">
+      <c r="CK2" s="96">
         <v>1001</v>
       </c>
-      <c r="CL2" s="107">
+      <c r="CL2" s="96">
         <v>1</v>
       </c>
-      <c r="CM2" s="107">
+      <c r="CM2" s="96">
         <v>1</v>
       </c>
-      <c r="CN2" s="107">
+      <c r="CN2" s="96">
         <v>2066665</v>
       </c>
-      <c r="CO2" s="107">
+      <c r="CO2" s="96">
         <v>2066665</v>
       </c>
-      <c r="CP2" s="107">
+      <c r="CP2" s="96">
         <v>100</v>
       </c>
-      <c r="CQ2" s="107">
+      <c r="CQ2" s="96">
         <v>100</v>
       </c>
-      <c r="CR2" s="107">
+      <c r="CR2" s="96">
         <v>2066665</v>
       </c>
-      <c r="CS2" s="107" t="s">
+      <c r="CS2" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="CT2" s="107">
+      <c r="CT2" s="96">
         <v>91</v>
       </c>
-      <c r="CU2" s="107">
+      <c r="CU2" s="96">
         <v>258</v>
       </c>
-      <c r="CV2" s="107" t="s">
+      <c r="CV2" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="CW2" s="108">
+      <c r="CW2" s="97">
         <v>26</v>
       </c>
-      <c r="CX2" s="107">
+      <c r="CX2" s="96">
         <v>1000</v>
       </c>
-      <c r="CY2" s="107">
+      <c r="CY2" s="96">
         <v>1</v>
       </c>
-      <c r="CZ2" s="107">
+      <c r="CZ2" s="96">
         <v>1</v>
       </c>
-      <c r="DA2" s="107">
+      <c r="DA2" s="96">
         <v>2068331</v>
       </c>
-      <c r="DB2" s="107">
+      <c r="DB2" s="96">
         <v>2068331</v>
       </c>
-      <c r="DC2" s="107">
+      <c r="DC2" s="96">
         <v>100</v>
       </c>
-      <c r="DD2" s="107">
+      <c r="DD2" s="96">
         <v>100</v>
       </c>
-      <c r="DE2" s="107">
+      <c r="DE2" s="96">
         <v>2068331</v>
       </c>
     </row>
     <row r="3" spans="1:109" x14ac:dyDescent="0.3">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="107">
+      <c r="B3" s="96">
         <v>1508949</v>
       </c>
-      <c r="C3" s="107">
+      <c r="C3" s="96">
         <v>26</v>
       </c>
-      <c r="D3" s="107">
+      <c r="D3" s="96">
         <v>452</v>
       </c>
-      <c r="E3" s="109">
+      <c r="E3" s="98">
         <v>4</v>
       </c>
-      <c r="F3" s="107" t="s">
+      <c r="F3" s="96" t="s">
         <v>226</v>
       </c>
-      <c r="G3" s="107">
+      <c r="G3" s="96">
         <v>1</v>
       </c>
-      <c r="H3" s="107">
+      <c r="H3" s="96">
         <v>258</v>
       </c>
-      <c r="I3" s="107" t="s">
+      <c r="I3" s="96" t="s">
         <v>226</v>
       </c>
-      <c r="J3" s="108">
+      <c r="J3" s="97">
         <v>26</v>
       </c>
-      <c r="K3" s="107">
+      <c r="K3" s="96">
         <v>5</v>
       </c>
-      <c r="L3" s="107">
+      <c r="L3" s="96">
         <v>1</v>
       </c>
-      <c r="M3" s="107">
+      <c r="M3" s="96">
         <v>1</v>
       </c>
-      <c r="N3" s="107">
+      <c r="N3" s="96">
         <v>2056669</v>
       </c>
-      <c r="O3" s="107">
+      <c r="O3" s="96">
         <v>2056669</v>
       </c>
-      <c r="P3" s="107">
+      <c r="P3" s="96">
         <v>100</v>
       </c>
-      <c r="Q3" s="107">
+      <c r="Q3" s="96">
         <v>100</v>
       </c>
-      <c r="R3" s="107">
+      <c r="R3" s="96">
         <v>2056669</v>
       </c>
-      <c r="S3" s="107" t="s">
+      <c r="S3" s="96" t="s">
         <v>227</v>
       </c>
-      <c r="T3" s="107">
+      <c r="T3" s="96">
         <v>2</v>
       </c>
-      <c r="U3" s="107">
+      <c r="U3" s="96">
         <v>258</v>
       </c>
-      <c r="V3" s="107" t="s">
+      <c r="V3" s="96" t="s">
         <v>227</v>
       </c>
-      <c r="W3" s="108">
+      <c r="W3" s="97">
         <v>26</v>
       </c>
-      <c r="X3" s="107">
+      <c r="X3" s="96">
         <v>10</v>
       </c>
-      <c r="Y3" s="107">
+      <c r="Y3" s="96">
         <v>1</v>
       </c>
-      <c r="Z3" s="107">
+      <c r="Z3" s="96">
         <v>1</v>
       </c>
-      <c r="AA3" s="107">
+      <c r="AA3" s="96">
         <v>2058335</v>
       </c>
-      <c r="AB3" s="107">
+      <c r="AB3" s="96">
         <v>2058335</v>
       </c>
-      <c r="AC3" s="107">
+      <c r="AC3" s="96">
         <v>100</v>
       </c>
-      <c r="AD3" s="107">
+      <c r="AD3" s="96">
         <v>100</v>
       </c>
-      <c r="AE3" s="107">
+      <c r="AE3" s="96">
         <v>2058335</v>
       </c>
-      <c r="AF3" s="107" t="s">
+      <c r="AF3" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="AG3" s="107">
+      <c r="AG3" s="96">
         <v>3</v>
       </c>
-      <c r="AH3" s="107">
+      <c r="AH3" s="96">
         <v>258</v>
       </c>
-      <c r="AI3" s="107" t="s">
+      <c r="AI3" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="AJ3" s="108">
+      <c r="AJ3" s="97">
         <v>26</v>
       </c>
-      <c r="AK3" s="107">
+      <c r="AK3" s="96">
         <v>15</v>
       </c>
-      <c r="AL3" s="107">
+      <c r="AL3" s="96">
         <v>1</v>
       </c>
-      <c r="AM3" s="107">
+      <c r="AM3" s="96">
         <v>1</v>
       </c>
-      <c r="AN3" s="107">
+      <c r="AN3" s="96">
         <v>2060001</v>
       </c>
-      <c r="AO3" s="107">
+      <c r="AO3" s="96">
         <v>2060001</v>
       </c>
-      <c r="AP3" s="107">
+      <c r="AP3" s="96">
         <v>100</v>
       </c>
-      <c r="AQ3" s="107">
+      <c r="AQ3" s="96">
         <v>100</v>
       </c>
-      <c r="AR3" s="107">
+      <c r="AR3" s="96">
         <v>2060001</v>
       </c>
-      <c r="AS3" s="107" t="s">
+      <c r="AS3" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="AT3" s="107">
+      <c r="AT3" s="96">
         <v>4</v>
       </c>
-      <c r="AU3" s="107">
+      <c r="AU3" s="96">
         <v>258</v>
       </c>
-      <c r="AV3" s="107" t="s">
+      <c r="AV3" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="AW3" s="108">
+      <c r="AW3" s="97">
         <v>26</v>
       </c>
-      <c r="AX3" s="107">
+      <c r="AX3" s="96">
         <v>20</v>
       </c>
-      <c r="AY3" s="107">
+      <c r="AY3" s="96">
         <v>1</v>
       </c>
-      <c r="AZ3" s="107">
+      <c r="AZ3" s="96">
         <v>1</v>
       </c>
-      <c r="BA3" s="107">
+      <c r="BA3" s="96">
         <v>2061667</v>
       </c>
-      <c r="BB3" s="107">
+      <c r="BB3" s="96">
         <v>2061667</v>
       </c>
-      <c r="BC3" s="107">
+      <c r="BC3" s="96">
         <v>100</v>
       </c>
-      <c r="BD3" s="107">
+      <c r="BD3" s="96">
         <v>100</v>
       </c>
-      <c r="BE3" s="107">
+      <c r="BE3" s="96">
         <v>2061667</v>
       </c>
-      <c r="BF3" s="107" t="s">
+      <c r="BF3" s="96" t="s">
         <v>230</v>
       </c>
-      <c r="BG3" s="107">
+      <c r="BG3" s="96">
         <v>5</v>
       </c>
-      <c r="BH3" s="107">
+      <c r="BH3" s="96">
         <v>258</v>
       </c>
-      <c r="BI3" s="107" t="s">
+      <c r="BI3" s="96" t="s">
         <v>230</v>
       </c>
-      <c r="BJ3" s="108">
+      <c r="BJ3" s="97">
         <v>26</v>
       </c>
-      <c r="BK3" s="107">
+      <c r="BK3" s="96">
         <v>25</v>
       </c>
-      <c r="BL3" s="107">
+      <c r="BL3" s="96">
         <v>1</v>
       </c>
-      <c r="BM3" s="107">
+      <c r="BM3" s="96">
         <v>1</v>
       </c>
-      <c r="BN3" s="107">
+      <c r="BN3" s="96">
         <v>2063333</v>
       </c>
-      <c r="BO3" s="107">
+      <c r="BO3" s="96">
         <v>2063333</v>
       </c>
-      <c r="BP3" s="107">
+      <c r="BP3" s="96">
         <v>100</v>
       </c>
-      <c r="BQ3" s="107">
+      <c r="BQ3" s="96">
         <v>100</v>
       </c>
-      <c r="BR3" s="107">
+      <c r="BR3" s="96">
         <v>2063333</v>
       </c>
-      <c r="BS3" s="107" t="s">
+      <c r="BS3" s="96" t="s">
         <v>231</v>
       </c>
-      <c r="BT3" s="107">
+      <c r="BT3" s="96">
         <v>6</v>
       </c>
-      <c r="BU3" s="107">
+      <c r="BU3" s="96">
         <v>258</v>
       </c>
-      <c r="BV3" s="107" t="s">
+      <c r="BV3" s="96" t="s">
         <v>231</v>
       </c>
-      <c r="BW3" s="108">
+      <c r="BW3" s="97">
         <v>26</v>
       </c>
-      <c r="BX3" s="107">
+      <c r="BX3" s="96">
         <v>30</v>
       </c>
-      <c r="BY3" s="107">
+      <c r="BY3" s="96">
         <v>1</v>
       </c>
-      <c r="BZ3" s="107">
+      <c r="BZ3" s="96">
         <v>1</v>
       </c>
-      <c r="CA3" s="107">
+      <c r="CA3" s="96">
         <v>2064999</v>
       </c>
-      <c r="CB3" s="107">
+      <c r="CB3" s="96">
         <v>2064999</v>
       </c>
-      <c r="CC3" s="107">
+      <c r="CC3" s="96">
         <v>100</v>
       </c>
-      <c r="CD3" s="107">
+      <c r="CD3" s="96">
         <v>100</v>
       </c>
-      <c r="CE3" s="107">
+      <c r="CE3" s="96">
         <v>2064999</v>
       </c>
-      <c r="CF3" s="107" t="s">
+      <c r="CF3" s="96" t="s">
         <v>232</v>
       </c>
-      <c r="CG3" s="107">
+      <c r="CG3" s="96">
         <v>7</v>
       </c>
-      <c r="CH3" s="107">
+      <c r="CH3" s="96">
         <v>258</v>
       </c>
-      <c r="CI3" s="107" t="s">
+      <c r="CI3" s="96" t="s">
         <v>232</v>
       </c>
-      <c r="CJ3" s="108">
+      <c r="CJ3" s="97">
         <v>26</v>
       </c>
-      <c r="CK3" s="107">
+      <c r="CK3" s="96">
         <v>35</v>
       </c>
-      <c r="CL3" s="107">
+      <c r="CL3" s="96">
         <v>1</v>
       </c>
-      <c r="CM3" s="107">
+      <c r="CM3" s="96">
         <v>1</v>
       </c>
-      <c r="CN3" s="107">
+      <c r="CN3" s="96">
         <v>2066665</v>
       </c>
-      <c r="CO3" s="107">
+      <c r="CO3" s="96">
         <v>2066665</v>
       </c>
-      <c r="CP3" s="107">
+      <c r="CP3" s="96">
         <v>100</v>
       </c>
-      <c r="CQ3" s="107">
+      <c r="CQ3" s="96">
         <v>100</v>
       </c>
-      <c r="CR3" s="107">
+      <c r="CR3" s="96">
         <v>2066665</v>
       </c>
-      <c r="CS3" s="107" t="s">
+      <c r="CS3" s="96" t="s">
         <v>233</v>
       </c>
-      <c r="CT3" s="107">
+      <c r="CT3" s="96">
         <v>8</v>
       </c>
-      <c r="CU3" s="107">
+      <c r="CU3" s="96">
         <v>258</v>
       </c>
-      <c r="CV3" s="107" t="s">
+      <c r="CV3" s="96" t="s">
         <v>233</v>
       </c>
-      <c r="CW3" s="108">
+      <c r="CW3" s="97">
         <v>26</v>
       </c>
-      <c r="CX3" s="107">
+      <c r="CX3" s="96">
         <v>40</v>
       </c>
-      <c r="CY3" s="107">
+      <c r="CY3" s="96">
         <v>1</v>
       </c>
-      <c r="CZ3" s="107">
+      <c r="CZ3" s="96">
         <v>1</v>
       </c>
-      <c r="DA3" s="107">
+      <c r="DA3" s="96">
         <v>2068331</v>
       </c>
-      <c r="DB3" s="107">
+      <c r="DB3" s="96">
         <v>2068331</v>
       </c>
-      <c r="DC3" s="107">
+      <c r="DC3" s="96">
         <v>100</v>
       </c>
-      <c r="DD3" s="107">
+      <c r="DD3" s="96">
         <v>100</v>
       </c>
-      <c r="DE3" s="107">
+      <c r="DE3" s="96">
         <v>2068331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improve remove header space trail
remove test template
trim space in excel header, avoid issue by user input cause script crash
</commit_message>
<xml_diff>
--- a/script_creater/5G_CDD.xlsx
+++ b/script_creater/5G_CDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\ephucle\tool_script\python\pythonlab\script_creater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358F9D08-0D55-49EF-B1FE-896D480EE4EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025E793D-43E0-48B4-A4A4-CBDA42F77EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1212" windowWidth="23040" windowHeight="11748" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="6" r:id="rId1"/>
@@ -4047,7 +4047,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>